<commit_message>
Auto commit 25-05-2025 14:41:22.56
</commit_message>
<xml_diff>
--- a/GWD Data/GI Works.xlsx
+++ b/GWD Data/GI Works.xlsx
@@ -1,15 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="130" yWindow="610" windowWidth="18880" windowHeight="6490"/>
-  </bookViews>
   <sheets>
-    <sheet name="GI Works" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="GI Works" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -164,101 +161,126 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="13.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Merriweather"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <color rgb="FF212529"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="13.0"/>
+      <color rgb="FF212529"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="13.0"/>
+      <color theme="1"/>
+      <name val="Merriweather"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <name val="Merriweather"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
+      <sz val="13.0"/>
+      <color rgb="FF000000"/>
       <name val="Merriweather"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF212529"/>
+        <bgColor rgb="FF212529"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE2E6"/>
+        <bgColor rgb="FFDEE2E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,104 +289,116 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+  <cellXfs count="30">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -554,29 +588,21 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <tabColor rgb="FF00FF00"/>
+    <tabColor rgb="FFFF00FF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="16384" width="12.6328125" style="6"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,27 +619,27 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+    <row r="2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
+    <row r="3">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3"/>
@@ -623,28 +649,28 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4">
       <c r="A4" s="10"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="11">
-        <v>100</v>
-      </c>
-      <c r="F4" s="12"/>
+      <c r="E4" s="12">
+        <v>100.0</v>
+      </c>
+      <c r="F4" s="13"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="10" t="s">
+    <row r="5">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3"/>
@@ -653,8 +679,8 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+    <row r="6">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3"/>
@@ -662,45 +688,45 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="14">
-        <v>8019</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="13" t="s">
+    <row r="7">
+      <c r="A7" s="17">
+        <v>8019.0</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="10" t="s">
+    <row r="8">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>1.05</v>
       </c>
-      <c r="E8" s="11">
-        <v>9000</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="E8" s="12">
+        <v>9000.0</v>
+      </c>
+      <c r="F8" s="19">
         <f>D8*E8</f>
         <v>9450</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+    <row r="9">
+      <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="3"/>
@@ -708,45 +734,45 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="14">
-        <v>2205</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="13" t="s">
+    <row r="10">
+      <c r="A10" s="17">
+        <v>2205.0</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="12"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="10" t="s">
+    <row r="11">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="12">
         <v>0.105</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="12">
         <v>145.72</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="19">
         <f>D11*E11</f>
-        <v>15.300599999999999</v>
-      </c>
-      <c r="G11" s="10" t="s">
+        <v>15.3006</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="13" t="s">
+    <row r="12">
+      <c r="A12" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="3"/>
@@ -754,144 +780,144 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="14">
-        <v>116</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="13" t="s">
+    <row r="13">
+      <c r="A13" s="17">
+        <v>116.0</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="12"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="10" t="s">
+    <row r="14">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="12">
         <v>0.5</v>
       </c>
-      <c r="E14" s="11">
-        <v>784</v>
-      </c>
-      <c r="F14" s="15">
+      <c r="E14" s="12">
+        <v>784.0</v>
+      </c>
+      <c r="F14" s="19">
         <f>E14*D14</f>
         <v>392</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="14">
-        <v>102</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="13" t="s">
+    <row r="15">
+      <c r="A15" s="17">
+        <v>102.0</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="12"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10" t="s">
+    <row r="16">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="12">
         <v>0.75</v>
       </c>
-      <c r="E16" s="11">
-        <v>784</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="E16" s="12">
+        <v>784.0</v>
+      </c>
+      <c r="F16" s="19">
         <f>E16*D16</f>
         <v>588</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" s="14">
-        <v>103</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="13" t="s">
+    <row r="17">
+      <c r="A17" s="17">
+        <v>103.0</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="12"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10" t="s">
+    <row r="18">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="11">
-        <v>1</v>
-      </c>
-      <c r="E18" s="11">
-        <v>714</v>
-      </c>
-      <c r="F18" s="15">
+      <c r="D18" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="12">
+        <v>714.0</v>
+      </c>
+      <c r="F18" s="19">
         <f>E18*D18</f>
         <v>714</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A19" s="14" t="s">
+    <row r="19">
+      <c r="A19" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="12"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="10" t="s">
+    <row r="20">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11">
-        <v>850</v>
-      </c>
-      <c r="E20" s="11">
-        <v>2</v>
-      </c>
-      <c r="F20" s="15">
+      <c r="D20" s="12">
+        <v>850.0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="F20" s="19">
         <f>D20*E20</f>
         <v>1700</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="13" t="s">
+    <row r="21">
+      <c r="A21" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="3"/>
@@ -899,189 +925,198 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="14" t="s">
+    <row r="22">
+      <c r="A22" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="12"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="10" t="s">
+    <row r="23">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="11">
-        <v>3</v>
-      </c>
-      <c r="E23" s="11">
+      <c r="D23" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E23" s="12">
         <v>48.19</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="19">
         <f>D23*E23</f>
         <v>144.57</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5">
-      <c r="A24" s="16" t="s">
+    <row r="24">
+      <c r="A24" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="11">
-        <v>100</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="D24" s="12">
+        <v>100.0</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="23">
         <f>SUM(F8,F11,F14,F16,F18,F20+F23)</f>
         <v>13003.8706</v>
       </c>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="16.5">
-      <c r="A25" s="16" t="s">
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="11">
-        <v>1</v>
-      </c>
-      <c r="E25" s="17" t="s">
+      <c r="D25" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="23">
         <f>F24/100</f>
-        <v>130.03870599999999</v>
-      </c>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="16.5">
-      <c r="A26" s="19" t="s">
+        <v>130.038706</v>
+      </c>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="18">
+      <c r="E26" s="23">
         <f>F25</f>
-        <v>130.03870599999999</v>
-      </c>
-      <c r="F26" s="18">
+        <v>130.038706</v>
+      </c>
+      <c r="F26" s="23">
         <f>E26/100</f>
-        <v>1.3003870599999998</v>
-      </c>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" ht="16.5">
-      <c r="A27" s="19" t="s">
+        <v>1.30038706</v>
+      </c>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18">
+      <c r="E27" s="24"/>
+      <c r="F27" s="23">
         <f>F25+F26</f>
-        <v>131.33909305999998</v>
-      </c>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" ht="16.5">
-      <c r="A28" s="19" t="s">
+        <v>131.3390931</v>
+      </c>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="18">
+      <c r="E28" s="23">
         <f>F27</f>
-        <v>131.33909305999998</v>
-      </c>
-      <c r="F28" s="18">
+        <v>131.3390931</v>
+      </c>
+      <c r="F28" s="23">
         <f>E28*0.15</f>
-        <v>19.700863958999996</v>
-      </c>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" ht="16.5">
-      <c r="A29" s="19" t="s">
+        <v>19.70086396</v>
+      </c>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18">
+      <c r="E29" s="24"/>
+      <c r="F29" s="23">
         <f>F27+F28</f>
-        <v>151.03995701899998</v>
-      </c>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" ht="16.5">
-      <c r="A30" s="19" t="s">
+        <v>151.039957</v>
+      </c>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="20">
-        <f>ROUND(F29,2)</f>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28">
+        <f>round(F29,2)</f>
         <v>151.04</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="29" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:E19"/>
@@ -1089,16 +1124,7 @@
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>